<commit_message>
update app script to make it more user friendly
</commit_message>
<xml_diff>
--- a/indicator_list.xlsx
+++ b/indicator_list.xlsx
@@ -1,248 +1,256 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\JMMI-yemen-dashboard\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE69BA5-08E5-444E-92C6-CE1DA592F567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
-  <si>
-    <t xml:space="preserve">Item</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Item2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Variable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMEB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I. Indices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMEB Cost</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="147">
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Item2</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>SMEB</t>
+  </si>
+  <si>
+    <t>I. Indices</t>
+  </si>
+  <si>
+    <t>SMEB Cost</t>
   </si>
   <si>
     <t xml:space="preserve"> YER</t>
   </si>
   <si>
-    <t xml:space="preserve">SMEB Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WASH_SMEB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WASH SMEB Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMEB Food</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Food_SMEB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Food SMEB Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parallel Exchange Rates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exchange_rates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">II. Currencies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YER to 1 USD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wheat Flour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wheat_flour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">III. Food items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price (1 Kg)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dry Beans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beans_dry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price (10 Pack)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canned Beans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beans_can</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price (15oz can)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lentils</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lentil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vegetable Oil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vegetable_oil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price (1 L)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sugar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sugar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">salt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potato</t>
-  </si>
-  <si>
-    <t xml:space="preserve">potato</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Onion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">onion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petrol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">petrol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IV. Fuels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diesel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diesel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bottled Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bottled_water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V. Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price (0.75 L)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treated Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">treated_water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price (10 L)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VI. Non-food items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price (100 g)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laundry Powder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">laundry_powder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sanitary Napkins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sanitary_napkins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bleach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bleach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price (Cubic m)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cooking gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cooking_gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water Trucking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cost_cubic_meter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price (18.8kg)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for food items were to increase by 100%, would you be able to respond to this increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for food items were to increase&lt;br&gt;by 100%, would you be able to respond to this&lt;br&gt;increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_increse_food_100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VI. Other indicators</t>
+    <t>SMEB Water</t>
+  </si>
+  <si>
+    <t>WASH_SMEB</t>
+  </si>
+  <si>
+    <t>WASH SMEB Cost</t>
+  </si>
+  <si>
+    <t>SMEB Food</t>
+  </si>
+  <si>
+    <t>Food_SMEB</t>
+  </si>
+  <si>
+    <t>Food SMEB Cost</t>
+  </si>
+  <si>
+    <t>Parallel Exchange Rates</t>
+  </si>
+  <si>
+    <t>exchange_rates</t>
+  </si>
+  <si>
+    <t>II. Currencies</t>
+  </si>
+  <si>
+    <t>YER to 1 USD</t>
+  </si>
+  <si>
+    <t>Wheat Flour</t>
+  </si>
+  <si>
+    <t>wheat_flour</t>
+  </si>
+  <si>
+    <t>III. Food items</t>
+  </si>
+  <si>
+    <t>Price (1 Kg)</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>rice</t>
+  </si>
+  <si>
+    <t>Dry Beans</t>
+  </si>
+  <si>
+    <t>beans_dry</t>
+  </si>
+  <si>
+    <t>Price (10 Pack)</t>
+  </si>
+  <si>
+    <t>Canned Beans</t>
+  </si>
+  <si>
+    <t>beans_can</t>
+  </si>
+  <si>
+    <t>Price (15oz can)</t>
+  </si>
+  <si>
+    <t>Lentils</t>
+  </si>
+  <si>
+    <t>lentil</t>
+  </si>
+  <si>
+    <t>Vegetable Oil</t>
+  </si>
+  <si>
+    <t>vegetable_oil</t>
+  </si>
+  <si>
+    <t>Price (1 L)</t>
+  </si>
+  <si>
+    <t>Sugar</t>
+  </si>
+  <si>
+    <t>sugar</t>
+  </si>
+  <si>
+    <t>Salt</t>
+  </si>
+  <si>
+    <t>salt</t>
+  </si>
+  <si>
+    <t>Potato</t>
+  </si>
+  <si>
+    <t>potato</t>
+  </si>
+  <si>
+    <t>Onion</t>
+  </si>
+  <si>
+    <t>onion</t>
+  </si>
+  <si>
+    <t>Petrol</t>
+  </si>
+  <si>
+    <t>petrol</t>
+  </si>
+  <si>
+    <t>IV. Fuels</t>
+  </si>
+  <si>
+    <t>Diesel</t>
+  </si>
+  <si>
+    <t>diesel</t>
+  </si>
+  <si>
+    <t>Bottled Water</t>
+  </si>
+  <si>
+    <t>bottled_water</t>
+  </si>
+  <si>
+    <t>V. Water</t>
+  </si>
+  <si>
+    <t>Price (0.75 L)</t>
+  </si>
+  <si>
+    <t>Treated Water</t>
+  </si>
+  <si>
+    <t>treated_water</t>
+  </si>
+  <si>
+    <t>Price (10 L)</t>
+  </si>
+  <si>
+    <t>Water Trucking</t>
+  </si>
+  <si>
+    <t>cost_cubic_meter</t>
+  </si>
+  <si>
+    <t>Price (18.8kg)</t>
+  </si>
+  <si>
+    <t>Soap</t>
+  </si>
+  <si>
+    <t>soap</t>
+  </si>
+  <si>
+    <t>VI. Non-food items</t>
+  </si>
+  <si>
+    <t>Price (100 g)</t>
+  </si>
+  <si>
+    <t>Laundry Powder</t>
+  </si>
+  <si>
+    <t>laundry_powder</t>
+  </si>
+  <si>
+    <t>Sanitary Napkins</t>
+  </si>
+  <si>
+    <t>sanitary_napkins</t>
+  </si>
+  <si>
+    <t>Bleach</t>
+  </si>
+  <si>
+    <t>bleach</t>
+  </si>
+  <si>
+    <t>Price (Cubic m)</t>
+  </si>
+  <si>
+    <t>Cooking gas</t>
+  </si>
+  <si>
+    <t>cooking_gas</t>
+  </si>
+  <si>
+    <t>If the demand for food items were to increase by 100%, would you be able to respond to this increase?</t>
+  </si>
+  <si>
+    <t>If the demand for food items were to increase&lt;br&gt;by 100%, would you be able to respond to this&lt;br&gt;increase?</t>
+  </si>
+  <si>
+    <t>mrk_increse_food_100</t>
+  </si>
+  <si>
+    <t>VII. Other indicators</t>
   </si>
   <si>
     <t xml:space="preserve">	% of traders</t>
@@ -251,216 +259,215 @@
     <t xml:space="preserve"> %</t>
   </si>
   <si>
-    <t xml:space="preserve">If the demand for food items were to increase by 50%, would you be able to respond to this increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for food items were to increase&lt;br&gt;by 50%, would you be able to respond to this&lt;br&gt;increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_increse_food_50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for fuel items were to increase by 100%, would you be able to respond to this increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for fuel items were to increase&lt;br&gt;by 100%, would you be able to respond to this&lt;br&gt;increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_increse_fuel_100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for fuel items were to increase by 50%, would you be able to respond to this increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for fuel items were to increase&lt;br&gt;by 50%, would you be able to respond to this&lt;br&gt;increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_increse_fuel_50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for WASH items were to increase by 100%, would you be able to respond to this increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for WASH items were to increase&lt;br&gt;by 100%, would you be able to respond to this&lt;br&gt;increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_increse_wash_100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for WASH items were to increase by 50%, would you be able to respond to this increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for WASH items were to increase&lt;br&gt;by 50%, would you be able to respond to this&lt;br&gt;increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_increse_wash_50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for water trucking were to increase by 100%, would you be able to respond to this increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for water trucking were to&lt;br&gt;increase by 100%, would you be able to&lt;br&gt;respond to this increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_increse_water_100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for water trucking were to increase by 50%, would you be able to respond to this increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for water trucking were to&lt;br&gt;increase by 50%, would you be able to respond&lt;br&gt;to this increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_increse_water_50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supply issues: Destruction/damage to storage capacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supply issues: Destruction/damage to storage&lt;br&gt;capacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_supply_issues.dmg_storage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supply issues: Movement restrictions (check points, curfews, roadblocks, etc)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supply issues: Movement restrictions (check&lt;br&gt;points, curfews, roadblocks, etc)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_supply_issues.move_restriction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Have supply routes changed in a way harmful to your business in the past 30 days?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Have supply routes changed in a way harmful&lt;br&gt;to your business in the past 30 days?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_supply_routes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling beans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_beans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling bleach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_bleach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling bottled water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_bottled_water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling cooking gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_cooking_gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling diesel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_diesel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling laundry powder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_laundry_powder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling lentil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_lentil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling onion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_onion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling petrol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_petrol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling potato</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_potato</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling rice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_rice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling salt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_salt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling sanitary napkins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_sanitary_napkins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling soap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_soap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling sugar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_sugar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling treated water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_treated_water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling vegetable oil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_vegetable_oil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling water trucking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_water_trucking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling wheat flour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_wheat_flour</t>
+    <t>If the demand for food items were to increase by 50%, would you be able to respond to this increase?</t>
+  </si>
+  <si>
+    <t>If the demand for food items were to increase&lt;br&gt;by 50%, would you be able to respond to this&lt;br&gt;increase?</t>
+  </si>
+  <si>
+    <t>mrk_increse_food_50</t>
+  </si>
+  <si>
+    <t>If the demand for fuel items were to increase by 100%, would you be able to respond to this increase?</t>
+  </si>
+  <si>
+    <t>If the demand for fuel items were to increase&lt;br&gt;by 100%, would you be able to respond to this&lt;br&gt;increase?</t>
+  </si>
+  <si>
+    <t>mrk_increse_fuel_100</t>
+  </si>
+  <si>
+    <t>If the demand for fuel items were to increase by 50%, would you be able to respond to this increase?</t>
+  </si>
+  <si>
+    <t>If the demand for fuel items were to increase&lt;br&gt;by 50%, would you be able to respond to this&lt;br&gt;increase?</t>
+  </si>
+  <si>
+    <t>mrk_increse_fuel_50</t>
+  </si>
+  <si>
+    <t>If the demand for WASH items were to increase by 100%, would you be able to respond to this increase?</t>
+  </si>
+  <si>
+    <t>If the demand for WASH items were to increase&lt;br&gt;by 100%, would you be able to respond to this&lt;br&gt;increase?</t>
+  </si>
+  <si>
+    <t>mrk_increse_wash_100</t>
+  </si>
+  <si>
+    <t>If the demand for WASH items were to increase by 50%, would you be able to respond to this increase?</t>
+  </si>
+  <si>
+    <t>If the demand for WASH items were to increase&lt;br&gt;by 50%, would you be able to respond to this&lt;br&gt;increase?</t>
+  </si>
+  <si>
+    <t>mrk_increse_wash_50</t>
+  </si>
+  <si>
+    <t>If the demand for water trucking were to increase by 100%, would you be able to respond to this increase?</t>
+  </si>
+  <si>
+    <t>If the demand for water trucking were to&lt;br&gt;increase by 100%, would you be able to&lt;br&gt;respond to this increase?</t>
+  </si>
+  <si>
+    <t>mrk_increse_water_100</t>
+  </si>
+  <si>
+    <t>If the demand for water trucking were to increase by 50%, would you be able to respond to this increase?</t>
+  </si>
+  <si>
+    <t>If the demand for water trucking were to&lt;br&gt;increase by 50%, would you be able to respond&lt;br&gt;to this increase?</t>
+  </si>
+  <si>
+    <t>mrk_increse_water_50</t>
+  </si>
+  <si>
+    <t>Supply issues: Destruction/damage to storage capacity</t>
+  </si>
+  <si>
+    <t>Supply issues: Destruction/damage to storage&lt;br&gt;capacity</t>
+  </si>
+  <si>
+    <t>mrk_supply_issues.dmg_storage</t>
+  </si>
+  <si>
+    <t>Supply issues: Movement restrictions (check points, curfews, roadblocks, etc)</t>
+  </si>
+  <si>
+    <t>Supply issues: Movement restrictions (check&lt;br&gt;points, curfews, roadblocks, etc)</t>
+  </si>
+  <si>
+    <t>mrk_supply_issues.move_restriction</t>
+  </si>
+  <si>
+    <t>Have supply routes changed in a way harmful to your business in the past 30 days?</t>
+  </si>
+  <si>
+    <t>Have supply routes changed in a way harmful&lt;br&gt;to your business in the past 30 days?</t>
+  </si>
+  <si>
+    <t>mrk_supply_routes</t>
+  </si>
+  <si>
+    <t>% of vendors selling beans</t>
+  </si>
+  <si>
+    <t>sell_beans</t>
+  </si>
+  <si>
+    <t>% of vendors selling bleach</t>
+  </si>
+  <si>
+    <t>sell_bleach</t>
+  </si>
+  <si>
+    <t>% of vendors selling bottled water</t>
+  </si>
+  <si>
+    <t>sell_bottled_water</t>
+  </si>
+  <si>
+    <t>% of vendors selling cooking gas</t>
+  </si>
+  <si>
+    <t>sell_cooking_gas</t>
+  </si>
+  <si>
+    <t>% of vendors selling diesel</t>
+  </si>
+  <si>
+    <t>sell_diesel</t>
+  </si>
+  <si>
+    <t>% of vendors selling laundry powder</t>
+  </si>
+  <si>
+    <t>sell_laundry_powder</t>
+  </si>
+  <si>
+    <t>% of vendors selling lentil</t>
+  </si>
+  <si>
+    <t>sell_lentil</t>
+  </si>
+  <si>
+    <t>% of vendors selling onion</t>
+  </si>
+  <si>
+    <t>sell_onion</t>
+  </si>
+  <si>
+    <t>% of vendors selling petrol</t>
+  </si>
+  <si>
+    <t>sell_petrol</t>
+  </si>
+  <si>
+    <t>% of vendors selling potato</t>
+  </si>
+  <si>
+    <t>sell_potato</t>
+  </si>
+  <si>
+    <t>% of vendors selling rice</t>
+  </si>
+  <si>
+    <t>sell_rice</t>
+  </si>
+  <si>
+    <t>% of vendors selling salt</t>
+  </si>
+  <si>
+    <t>sell_salt</t>
+  </si>
+  <si>
+    <t>% of vendors selling sanitary napkins</t>
+  </si>
+  <si>
+    <t>sell_sanitary_napkins</t>
+  </si>
+  <si>
+    <t>% of vendors selling soap</t>
+  </si>
+  <si>
+    <t>sell_soap</t>
+  </si>
+  <si>
+    <t>% of vendors selling sugar</t>
+  </si>
+  <si>
+    <t>sell_sugar</t>
+  </si>
+  <si>
+    <t>% of vendors selling treated water</t>
+  </si>
+  <si>
+    <t>sell_treated_water</t>
+  </si>
+  <si>
+    <t>% of vendors selling vegetable oil</t>
+  </si>
+  <si>
+    <t>sell_vegetable_oil</t>
+  </si>
+  <si>
+    <t>% of vendors selling water trucking</t>
+  </si>
+  <si>
+    <t>sell_water_trucking</t>
+  </si>
+  <si>
+    <t>% of vendors selling wheat flour</t>
+  </si>
+  <si>
+    <t>sell_wheat_flour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -496,6 +503,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -777,14 +793,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="7" width="27.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -804,7 +825,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -824,7 +845,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -844,7 +865,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -864,7 +885,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -884,7 +905,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -904,7 +925,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -924,7 +945,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -944,7 +965,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -964,7 +985,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -984,7 +1005,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1004,7 +1025,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -1024,7 +1045,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1044,7 +1065,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1064,7 +1085,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1084,7 +1105,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1104,7 +1125,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1124,7 +1145,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -1144,7 +1165,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1164,7 +1185,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1175,76 +1196,76 @@
         <v>58</v>
       </c>
       <c r="D20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" t="s">
         <v>59</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>60</v>
       </c>
-      <c r="F20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
         <v>61</v>
       </c>
-      <c r="B21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>62</v>
       </c>
-      <c r="D21" t="s">
-        <v>59</v>
-      </c>
       <c r="E21" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" t="s">
         <v>63</v>
       </c>
-      <c r="B22" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" t="s">
-        <v>59</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" t="s">
         <v>28</v>
       </c>
-      <c r="F22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" t="s">
-        <v>67</v>
-      </c>
       <c r="F23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -1255,36 +1276,36 @@
         <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E24" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" t="s">
         <v>36</v>
       </c>
-      <c r="F24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25" t="s">
-        <v>72</v>
-      </c>
       <c r="F25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>73</v>
       </c>
@@ -1304,7 +1325,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -1324,7 +1345,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -1344,7 +1365,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>85</v>
       </c>
@@ -1364,7 +1385,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>88</v>
       </c>
@@ -1384,7 +1405,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>91</v>
       </c>
@@ -1404,7 +1425,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -1424,7 +1445,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -1444,7 +1465,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -1464,7 +1485,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -1484,7 +1505,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>106</v>
       </c>
@@ -1504,7 +1525,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>109</v>
       </c>
@@ -1524,7 +1545,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>111</v>
       </c>
@@ -1544,7 +1565,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>113</v>
       </c>
@@ -1564,7 +1585,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>115</v>
       </c>
@@ -1584,7 +1605,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>117</v>
       </c>
@@ -1604,7 +1625,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>119</v>
       </c>
@@ -1624,7 +1645,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>121</v>
       </c>
@@ -1644,7 +1665,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>123</v>
       </c>
@@ -1664,7 +1685,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>125</v>
       </c>
@@ -1684,7 +1705,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>127</v>
       </c>
@@ -1704,7 +1725,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>129</v>
       </c>
@@ -1724,7 +1745,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>131</v>
       </c>
@@ -1744,7 +1765,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>133</v>
       </c>
@@ -1764,7 +1785,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>135</v>
       </c>
@@ -1784,7 +1805,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>137</v>
       </c>
@@ -1804,7 +1825,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>139</v>
       </c>
@@ -1824,7 +1845,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>141</v>
       </c>
@@ -1844,7 +1865,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>143</v>
       </c>
@@ -1864,7 +1885,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>145</v>
       </c>
@@ -1886,6 +1907,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Integrated HQ suggestions - use variable labels for plot and explorer tabs + adapt the legend for the map
</commit_message>
<xml_diff>
--- a/indicator_list.xlsx
+++ b/indicator_list.xlsx
@@ -1,299 +1,308 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\JMMI-yemen-dashboard\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62BB1DA-011B-42CE-944D-22CE93841E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="169">
-  <si>
-    <t xml:space="preserve">Item</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Item2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Variable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMEB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I. Indices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMEB Cost</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="188">
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Item2</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>SMEB</t>
+  </si>
+  <si>
+    <t>I. Indices</t>
+  </si>
+  <si>
+    <t>SMEB Cost</t>
   </si>
   <si>
     <t xml:space="preserve"> YER</t>
   </si>
   <si>
-    <t xml:space="preserve">SMEB Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WASH_SMEB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WASH SMEB Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMEB Food</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Food_SMEB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Food SMEB Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily wage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">daily_wage_rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily wage (YER)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parallel Exchange Rates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exchange_rates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">II. Currencies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YER to 1 USD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wheat Flour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wheat_flour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">III. Food items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price (1 Kg)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dry Beans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beans_dry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price (10 Pack)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canned Beans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beans_can</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price (15oz can)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lentils</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lentil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vegetable Oil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vegetable_oil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price (1 L)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sugar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sugar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">salt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potato</t>
-  </si>
-  <si>
-    <t xml:space="preserve">potato</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Onion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">onion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petrol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">petrol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IV. Fuels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diesel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diesel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bottled Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bottled_water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V. Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price (0.75 L)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treated Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">treated_water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price (10 L)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water Trucking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cost_cubic_meter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price (18.8kg)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VI. Non-food items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price (100 g)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laundry Powder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">laundry_powder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sanitary Napkins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sanitary_napkins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bleach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bleach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price (Cubic m)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cooking gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cooking_gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For an order of 10 km for the full truck, what is the additional cost of delivery? (in YER)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For an order of 10 km for the full truck,&lt;br&gt;what is the additional cost of delivery? (in&lt;br&gt;YER)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">additional_cost_10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VII. Other indicators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost (YER)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For an order of 15 km for the full truck, what is the additional cost of delivery? (in YER)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For an order of 15 km for the full truck,&lt;br&gt;what is the additional cost of delivery? (in&lt;br&gt;YER)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">additional_cost_20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For an order of 20 km for the full truck, what is the additional cost of delivery? (in YER)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For an order of 20 km for the full truck,&lt;br&gt;what is the additional cost of delivery? (in&lt;br&gt;YER)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">additional_cost_30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For an order of 5 km for the full truck, what is the additional cost of delivery? (in YER)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For an order of 5 km for the full truck, what&lt;br&gt;is the additional cost of delivery? (in YER)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">additional_cost_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do you charge different prices depending on the distance you must travel to deliver water?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do you charge different prices depending&lt;br&gt;on the distance you must travel to deliver&lt;br&gt;water?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">distance_price</t>
+    <t>SMEB Water</t>
+  </si>
+  <si>
+    <t>WASH_SMEB</t>
+  </si>
+  <si>
+    <t>WASH SMEB Cost</t>
+  </si>
+  <si>
+    <t>SMEB Food</t>
+  </si>
+  <si>
+    <t>Food_SMEB</t>
+  </si>
+  <si>
+    <t>Food SMEB Cost</t>
+  </si>
+  <si>
+    <t>Daily wage</t>
+  </si>
+  <si>
+    <t>daily_wage_rate</t>
+  </si>
+  <si>
+    <t>Daily wage (YER)</t>
+  </si>
+  <si>
+    <t>Parallel Exchange Rates</t>
+  </si>
+  <si>
+    <t>exchange_rates</t>
+  </si>
+  <si>
+    <t>II. Currencies</t>
+  </si>
+  <si>
+    <t>YER to 1 USD</t>
+  </si>
+  <si>
+    <t>Wheat Flour</t>
+  </si>
+  <si>
+    <t>wheat_flour</t>
+  </si>
+  <si>
+    <t>III. Food items</t>
+  </si>
+  <si>
+    <t>Price (1 Kg)</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>rice</t>
+  </si>
+  <si>
+    <t>Dry Beans</t>
+  </si>
+  <si>
+    <t>beans_dry</t>
+  </si>
+  <si>
+    <t>Price (10 Pack)</t>
+  </si>
+  <si>
+    <t>Canned Beans</t>
+  </si>
+  <si>
+    <t>beans_can</t>
+  </si>
+  <si>
+    <t>Price (15oz can)</t>
+  </si>
+  <si>
+    <t>Lentils</t>
+  </si>
+  <si>
+    <t>lentil</t>
+  </si>
+  <si>
+    <t>Vegetable Oil</t>
+  </si>
+  <si>
+    <t>vegetable_oil</t>
+  </si>
+  <si>
+    <t>Price (1 L)</t>
+  </si>
+  <si>
+    <t>Sugar</t>
+  </si>
+  <si>
+    <t>sugar</t>
+  </si>
+  <si>
+    <t>Salt</t>
+  </si>
+  <si>
+    <t>salt</t>
+  </si>
+  <si>
+    <t>Potato</t>
+  </si>
+  <si>
+    <t>potato</t>
+  </si>
+  <si>
+    <t>Onion</t>
+  </si>
+  <si>
+    <t>onion</t>
+  </si>
+  <si>
+    <t>Petrol</t>
+  </si>
+  <si>
+    <t>petrol</t>
+  </si>
+  <si>
+    <t>IV. Fuels</t>
+  </si>
+  <si>
+    <t>Diesel</t>
+  </si>
+  <si>
+    <t>diesel</t>
+  </si>
+  <si>
+    <t>Bottled Water</t>
+  </si>
+  <si>
+    <t>bottled_water</t>
+  </si>
+  <si>
+    <t>V. Water</t>
+  </si>
+  <si>
+    <t>Price (0.75 L)</t>
+  </si>
+  <si>
+    <t>Treated Water</t>
+  </si>
+  <si>
+    <t>treated_water</t>
+  </si>
+  <si>
+    <t>Price (10 L)</t>
+  </si>
+  <si>
+    <t>Water Trucking</t>
+  </si>
+  <si>
+    <t>cost_cubic_meter</t>
+  </si>
+  <si>
+    <t>Price (18.8kg)</t>
+  </si>
+  <si>
+    <t>Soap</t>
+  </si>
+  <si>
+    <t>soap</t>
+  </si>
+  <si>
+    <t>VI. Non-food items</t>
+  </si>
+  <si>
+    <t>Price (100 g)</t>
+  </si>
+  <si>
+    <t>Laundry Powder</t>
+  </si>
+  <si>
+    <t>laundry_powder</t>
+  </si>
+  <si>
+    <t>Sanitary Napkins</t>
+  </si>
+  <si>
+    <t>sanitary_napkins</t>
+  </si>
+  <si>
+    <t>Bleach</t>
+  </si>
+  <si>
+    <t>bleach</t>
+  </si>
+  <si>
+    <t>Price (Cubic m)</t>
+  </si>
+  <si>
+    <t>Cooking gas</t>
+  </si>
+  <si>
+    <t>cooking_gas</t>
+  </si>
+  <si>
+    <t>For an order of 10 km for the full truck, what is the additional cost of delivery? (in YER)</t>
+  </si>
+  <si>
+    <t>For an order of 10 km for the full truck,&lt;br&gt;what is the additional cost of delivery? (in&lt;br&gt;YER)</t>
+  </si>
+  <si>
+    <t>additional_cost_10</t>
+  </si>
+  <si>
+    <t>VII. Other indicators</t>
+  </si>
+  <si>
+    <t>Cost (YER)</t>
+  </si>
+  <si>
+    <t>YER</t>
+  </si>
+  <si>
+    <t>For an order of 15 km for the full truck, what is the additional cost of delivery? (in YER)</t>
+  </si>
+  <si>
+    <t>For an order of 15 km for the full truck,&lt;br&gt;what is the additional cost of delivery? (in&lt;br&gt;YER)</t>
+  </si>
+  <si>
+    <t>additional_cost_20</t>
+  </si>
+  <si>
+    <t>For an order of 20 km for the full truck, what is the additional cost of delivery? (in YER)</t>
+  </si>
+  <si>
+    <t>For an order of 20 km for the full truck,&lt;br&gt;what is the additional cost of delivery? (in&lt;br&gt;YER)</t>
+  </si>
+  <si>
+    <t>additional_cost_30</t>
+  </si>
+  <si>
+    <t>For an order of 5 km for the full truck, what is the additional cost of delivery? (in YER)</t>
+  </si>
+  <si>
+    <t>For an order of 5 km for the full truck, what&lt;br&gt;is the additional cost of delivery? (in YER)</t>
+  </si>
+  <si>
+    <t>additional_cost_5</t>
+  </si>
+  <si>
+    <t>Do you charge different prices depending on the distance you must travel to deliver water?</t>
+  </si>
+  <si>
+    <t>Do you charge different prices depending&lt;br&gt;on the distance you must travel to deliver&lt;br&gt;water?</t>
+  </si>
+  <si>
+    <t>distance_price</t>
   </si>
   <si>
     <t xml:space="preserve">	% of traders</t>
@@ -302,231 +311,287 @@
     <t xml:space="preserve"> %</t>
   </si>
   <si>
-    <t xml:space="preserve">If the demand for food items were to increase by 100%, would you be able to respond to this increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for food items were to increase&lt;br&gt;by 100%, would you be able to respond to this&lt;br&gt;increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_increse_food_100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for food items were to increase by 50%, would you be able to respond to this increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for food items were to increase&lt;br&gt;by 50%, would you be able to respond to this&lt;br&gt;increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_increse_food_50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for fuel items were to increase by 100%, would you be able to respond to this increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for fuel items were to increase&lt;br&gt;by 100%, would you be able to respond to this&lt;br&gt;increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_increse_fuel_100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for fuel items were to increase by 50%, would you be able to respond to this increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for fuel items were to increase&lt;br&gt;by 50%, would you be able to respond to this&lt;br&gt;increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_increse_fuel_50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for WASH items were to increase by 100%, would you be able to respond to this increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for WASH items were to increase&lt;br&gt;by 100%, would you be able to respond to this&lt;br&gt;increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_increse_wash_100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for WASH items were to increase by 50%, would you be able to respond to this increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for WASH items were to increase&lt;br&gt;by 50%, would you be able to respond to this&lt;br&gt;increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_increse_wash_50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for water trucking were to increase by 100%, would you be able to respond to this increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for water trucking were to&lt;br&gt;increase by 100%, would you be able to&lt;br&gt;respond to this increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_increse_water_100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for water trucking were to increase by 50%, would you be able to respond to this increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the demand for water trucking were to&lt;br&gt;increase by 50%, would you be able to respond&lt;br&gt;to this increase?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_increse_water_50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supply issues: Destruction/damage to storage capacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supply issues: Destruction/damage to storage&lt;br&gt;capacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_supply_issues.dmg_storage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supply issues: Movement restrictions (check points, curfews, roadblocks, etc)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supply issues: Movement restrictions (check&lt;br&gt;points, curfews, roadblocks, etc)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_supply_issues.move_restriction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Have supply routes changed in a way harmful to your business in the past 30 days?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Have supply routes changed in a way harmful&lt;br&gt;to your business in the past 30 days?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrk_supply_routes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling beans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_beans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling bleach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_bleach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling bottled water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_bottled_water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling cooking gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_cooking_gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling diesel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_diesel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling laundry powder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_laundry_powder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling lentil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_lentil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling onion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_onion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling petrol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_petrol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling potato</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_potato</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling rice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_rice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling salt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_salt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling sanitary napkins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_sanitary_napkins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling soap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_soap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling sugar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_sugar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling treated water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_treated_water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling vegetable oil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_vegetable_oil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling water trucking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_water_trucking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of vendors selling wheat flour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sell_wheat_flour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is the water from water trucking chlorinated?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">water_chlorinated</t>
+    <t>If the demand for food items were to increase by 100%, would you be able to respond to this increase?</t>
+  </si>
+  <si>
+    <t>If the demand for food items were to increase&lt;br&gt;by 100%, would you be able to respond to this&lt;br&gt;increase?</t>
+  </si>
+  <si>
+    <t>mrk_increse_food_100</t>
+  </si>
+  <si>
+    <t>If the demand for food items were to increase by 50%, would you be able to respond to this increase?</t>
+  </si>
+  <si>
+    <t>If the demand for food items were to increase&lt;br&gt;by 50%, would you be able to respond to this&lt;br&gt;increase?</t>
+  </si>
+  <si>
+    <t>mrk_increse_food_50</t>
+  </si>
+  <si>
+    <t>If the demand for fuel items were to increase by 100%, would you be able to respond to this increase?</t>
+  </si>
+  <si>
+    <t>If the demand for fuel items were to increase&lt;br&gt;by 100%, would you be able to respond to this&lt;br&gt;increase?</t>
+  </si>
+  <si>
+    <t>mrk_increse_fuel_100</t>
+  </si>
+  <si>
+    <t>If the demand for fuel items were to increase by 50%, would you be able to respond to this increase?</t>
+  </si>
+  <si>
+    <t>If the demand for fuel items were to increase&lt;br&gt;by 50%, would you be able to respond to this&lt;br&gt;increase?</t>
+  </si>
+  <si>
+    <t>mrk_increse_fuel_50</t>
+  </si>
+  <si>
+    <t>If the demand for WASH items were to increase by 100%, would you be able to respond to this increase?</t>
+  </si>
+  <si>
+    <t>If the demand for WASH items were to increase&lt;br&gt;by 100%, would you be able to respond to this&lt;br&gt;increase?</t>
+  </si>
+  <si>
+    <t>mrk_increse_wash_100</t>
+  </si>
+  <si>
+    <t>If the demand for WASH items were to increase by 50%, would you be able to respond to this increase?</t>
+  </si>
+  <si>
+    <t>If the demand for WASH items were to increase&lt;br&gt;by 50%, would you be able to respond to this&lt;br&gt;increase?</t>
+  </si>
+  <si>
+    <t>mrk_increse_wash_50</t>
+  </si>
+  <si>
+    <t>If the demand for water trucking were to increase by 100%, would you be able to respond to this increase?</t>
+  </si>
+  <si>
+    <t>If the demand for water trucking were to&lt;br&gt;increase by 100%, would you be able to&lt;br&gt;respond to this increase?</t>
+  </si>
+  <si>
+    <t>mrk_increse_water_100</t>
+  </si>
+  <si>
+    <t>If the demand for water trucking were to increase by 50%, would you be able to respond to this increase?</t>
+  </si>
+  <si>
+    <t>If the demand for water trucking were to&lt;br&gt;increase by 50%, would you be able to respond&lt;br&gt;to this increase?</t>
+  </si>
+  <si>
+    <t>mrk_increse_water_50</t>
+  </si>
+  <si>
+    <t>Supply issues: Destruction/damage to storage capacity</t>
+  </si>
+  <si>
+    <t>Supply issues: Destruction/damage to storage&lt;br&gt;capacity</t>
+  </si>
+  <si>
+    <t>mrk_supply_issues.dmg_storage</t>
+  </si>
+  <si>
+    <t>Supply issues: Movement restrictions (check points, curfews, roadblocks, etc)</t>
+  </si>
+  <si>
+    <t>Supply issues: Movement restrictions (check&lt;br&gt;points, curfews, roadblocks, etc)</t>
+  </si>
+  <si>
+    <t>mrk_supply_issues.move_restriction</t>
+  </si>
+  <si>
+    <t>Have supply routes changed in a way harmful to your business in the past 30 days?</t>
+  </si>
+  <si>
+    <t>Have supply routes changed in a way harmful&lt;br&gt;to your business in the past 30 days?</t>
+  </si>
+  <si>
+    <t>mrk_supply_routes</t>
+  </si>
+  <si>
+    <t>% of vendors selling beans</t>
+  </si>
+  <si>
+    <t>sell_beans</t>
+  </si>
+  <si>
+    <t>% of vendors selling bleach</t>
+  </si>
+  <si>
+    <t>sell_bleach</t>
+  </si>
+  <si>
+    <t>% of vendors selling bottled water</t>
+  </si>
+  <si>
+    <t>sell_bottled_water</t>
+  </si>
+  <si>
+    <t>% of vendors selling cooking gas</t>
+  </si>
+  <si>
+    <t>sell_cooking_gas</t>
+  </si>
+  <si>
+    <t>% of vendors selling diesel</t>
+  </si>
+  <si>
+    <t>sell_diesel</t>
+  </si>
+  <si>
+    <t>% of vendors selling laundry powder</t>
+  </si>
+  <si>
+    <t>sell_laundry_powder</t>
+  </si>
+  <si>
+    <t>% of vendors selling lentil</t>
+  </si>
+  <si>
+    <t>sell_lentil</t>
+  </si>
+  <si>
+    <t>% of vendors selling onion</t>
+  </si>
+  <si>
+    <t>sell_onion</t>
+  </si>
+  <si>
+    <t>% of vendors selling petrol</t>
+  </si>
+  <si>
+    <t>sell_petrol</t>
+  </si>
+  <si>
+    <t>% of vendors selling potato</t>
+  </si>
+  <si>
+    <t>sell_potato</t>
+  </si>
+  <si>
+    <t>% of vendors selling rice</t>
+  </si>
+  <si>
+    <t>sell_rice</t>
+  </si>
+  <si>
+    <t>% of vendors selling salt</t>
+  </si>
+  <si>
+    <t>sell_salt</t>
+  </si>
+  <si>
+    <t>% of vendors selling sanitary napkins</t>
+  </si>
+  <si>
+    <t>sell_sanitary_napkins</t>
+  </si>
+  <si>
+    <t>% of vendors selling soap</t>
+  </si>
+  <si>
+    <t>sell_soap</t>
+  </si>
+  <si>
+    <t>% of vendors selling sugar</t>
+  </si>
+  <si>
+    <t>sell_sugar</t>
+  </si>
+  <si>
+    <t>% of vendors selling treated water</t>
+  </si>
+  <si>
+    <t>sell_treated_water</t>
+  </si>
+  <si>
+    <t>% of vendors selling vegetable oil</t>
+  </si>
+  <si>
+    <t>sell_vegetable_oil</t>
+  </si>
+  <si>
+    <t>% of vendors selling water trucking</t>
+  </si>
+  <si>
+    <t>sell_water_trucking</t>
+  </si>
+  <si>
+    <t>% of vendors selling wheat flour</t>
+  </si>
+  <si>
+    <t>sell_wheat_flour</t>
+  </si>
+  <si>
+    <t>Is the water from water trucking chlorinated?</t>
+  </si>
+  <si>
+    <t>water_chlorinated</t>
+  </si>
+  <si>
+    <t>food_gov_origin</t>
+  </si>
+  <si>
+    <t>wash_gov_origin</t>
+  </si>
+  <si>
+    <t>fuel_gov_origin</t>
+  </si>
+  <si>
+    <t>district_ID</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>government_ID</t>
+  </si>
+  <si>
+    <t>Governorate</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>jmmi</t>
+  </si>
+  <si>
+    <t>Meta columns</t>
+  </si>
+  <si>
+    <t>From which governorate is the majority of fuel items being transported from?</t>
+  </si>
+  <si>
+    <t>From which governorate is the majority of wash items being transported from?</t>
+  </si>
+  <si>
+    <t>From which governorate is the majority of food items being transported from?</t>
+  </si>
+  <si>
+    <t>From which governorate is the majority&lt;br&gt; of fuel items being transported from?</t>
+  </si>
+  <si>
+    <t>From which governorate is the majority&lt;br&gt; of wash items being transported from?</t>
+  </si>
+  <si>
+    <t>From which governorate is the majority&lt;br&gt; of food items being transported from?</t>
+  </si>
+  <si>
+    <t>JMMI Round</t>
+  </si>
+  <si>
+    <t>Governorate Pcode</t>
+  </si>
+  <si>
+    <t>District Pcode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -562,6 +627,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -843,14 +917,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B62"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="38" customWidth="1"/>
+    <col min="3" max="3" width="31.5546875" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -870,7 +952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -890,7 +972,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -910,7 +992,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -930,7 +1012,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -950,7 +1032,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -970,7 +1052,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -990,7 +1072,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1010,7 +1092,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1030,7 +1112,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1050,7 +1132,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1070,7 +1152,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -1090,7 +1172,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1110,7 +1192,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1130,7 +1212,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -1150,7 +1232,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -1170,7 +1252,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1190,7 +1272,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -1210,7 +1292,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1230,7 +1312,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1250,7 +1332,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -1270,7 +1352,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -1290,7 +1372,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -1310,7 +1392,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -1330,7 +1412,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -1350,7 +1432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -1370,7 +1452,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>76</v>
       </c>
@@ -1390,7 +1472,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -1410,7 +1492,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>85</v>
       </c>
@@ -1430,7 +1512,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>88</v>
       </c>
@@ -1450,7 +1532,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>91</v>
       </c>
@@ -1470,7 +1552,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>96</v>
       </c>
@@ -1490,7 +1572,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>99</v>
       </c>
@@ -1510,7 +1592,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>102</v>
       </c>
@@ -1530,7 +1612,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>105</v>
       </c>
@@ -1550,7 +1632,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>108</v>
       </c>
@@ -1570,7 +1652,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>111</v>
       </c>
@@ -1590,7 +1672,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>114</v>
       </c>
@@ -1610,7 +1692,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>117</v>
       </c>
@@ -1630,7 +1712,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>120</v>
       </c>
@@ -1650,7 +1732,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>123</v>
       </c>
@@ -1670,7 +1752,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>126</v>
       </c>
@@ -1690,7 +1772,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>129</v>
       </c>
@@ -1710,7 +1792,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>131</v>
       </c>
@@ -1730,7 +1812,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>133</v>
       </c>
@@ -1750,7 +1832,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>135</v>
       </c>
@@ -1770,7 +1852,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>137</v>
       </c>
@@ -1790,7 +1872,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>139</v>
       </c>
@@ -1810,7 +1892,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>141</v>
       </c>
@@ -1830,7 +1912,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>143</v>
       </c>
@@ -1850,7 +1932,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>145</v>
       </c>
@@ -1870,7 +1952,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>147</v>
       </c>
@@ -1890,7 +1972,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>149</v>
       </c>
@@ -1910,7 +1992,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>151</v>
       </c>
@@ -1930,7 +2012,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>153</v>
       </c>
@@ -1950,7 +2032,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>155</v>
       </c>
@@ -1970,7 +2052,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>157</v>
       </c>
@@ -1990,7 +2072,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>159</v>
       </c>
@@ -2010,7 +2092,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>161</v>
       </c>
@@ -2030,7 +2112,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>163</v>
       </c>
@@ -2050,7 +2132,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>165</v>
       </c>
@@ -2070,7 +2152,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>167</v>
       </c>
@@ -2092,6 +2174,1021 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B199B668-28AF-4688-9C4C-70534225EB9D}">
+  <dimension ref="A1:D71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="58.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" t="s">
+        <v>98</v>
+      </c>
+      <c r="D38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>99</v>
+      </c>
+      <c r="B39" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>108</v>
+      </c>
+      <c r="B42" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>114</v>
+      </c>
+      <c r="B44" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" t="s">
+        <v>116</v>
+      </c>
+      <c r="D44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>117</v>
+      </c>
+      <c r="B45" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" t="s">
+        <v>119</v>
+      </c>
+      <c r="D45" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B46" t="s">
+        <v>121</v>
+      </c>
+      <c r="C46" t="s">
+        <v>122</v>
+      </c>
+      <c r="D46" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>123</v>
+      </c>
+      <c r="B47" t="s">
+        <v>124</v>
+      </c>
+      <c r="C47" t="s">
+        <v>125</v>
+      </c>
+      <c r="D47" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>126</v>
+      </c>
+      <c r="B48" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48" t="s">
+        <v>128</v>
+      </c>
+      <c r="D48" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>129</v>
+      </c>
+      <c r="B49" t="s">
+        <v>129</v>
+      </c>
+      <c r="C49" t="s">
+        <v>130</v>
+      </c>
+      <c r="D49" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>131</v>
+      </c>
+      <c r="B50" t="s">
+        <v>131</v>
+      </c>
+      <c r="C50" t="s">
+        <v>132</v>
+      </c>
+      <c r="D50" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>133</v>
+      </c>
+      <c r="B51" t="s">
+        <v>133</v>
+      </c>
+      <c r="C51" t="s">
+        <v>134</v>
+      </c>
+      <c r="D51" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>135</v>
+      </c>
+      <c r="B52" t="s">
+        <v>135</v>
+      </c>
+      <c r="C52" t="s">
+        <v>136</v>
+      </c>
+      <c r="D52" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>137</v>
+      </c>
+      <c r="B53" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53" t="s">
+        <v>138</v>
+      </c>
+      <c r="D53" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>139</v>
+      </c>
+      <c r="B54" t="s">
+        <v>139</v>
+      </c>
+      <c r="C54" t="s">
+        <v>140</v>
+      </c>
+      <c r="D54" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>141</v>
+      </c>
+      <c r="B55" t="s">
+        <v>141</v>
+      </c>
+      <c r="C55" t="s">
+        <v>142</v>
+      </c>
+      <c r="D55" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>143</v>
+      </c>
+      <c r="B56" t="s">
+        <v>143</v>
+      </c>
+      <c r="C56" t="s">
+        <v>144</v>
+      </c>
+      <c r="D56" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>145</v>
+      </c>
+      <c r="B57" t="s">
+        <v>145</v>
+      </c>
+      <c r="C57" t="s">
+        <v>146</v>
+      </c>
+      <c r="D57" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>147</v>
+      </c>
+      <c r="B58" t="s">
+        <v>147</v>
+      </c>
+      <c r="C58" t="s">
+        <v>148</v>
+      </c>
+      <c r="D58" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>149</v>
+      </c>
+      <c r="B59" t="s">
+        <v>149</v>
+      </c>
+      <c r="C59" t="s">
+        <v>150</v>
+      </c>
+      <c r="D59" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>151</v>
+      </c>
+      <c r="B60" t="s">
+        <v>151</v>
+      </c>
+      <c r="C60" t="s">
+        <v>152</v>
+      </c>
+      <c r="D60" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>153</v>
+      </c>
+      <c r="B61" t="s">
+        <v>153</v>
+      </c>
+      <c r="C61" t="s">
+        <v>154</v>
+      </c>
+      <c r="D61" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>155</v>
+      </c>
+      <c r="B62" t="s">
+        <v>155</v>
+      </c>
+      <c r="C62" t="s">
+        <v>156</v>
+      </c>
+      <c r="D62" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>157</v>
+      </c>
+      <c r="B63" t="s">
+        <v>157</v>
+      </c>
+      <c r="C63" t="s">
+        <v>158</v>
+      </c>
+      <c r="D63" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>159</v>
+      </c>
+      <c r="B64" t="s">
+        <v>159</v>
+      </c>
+      <c r="C64" t="s">
+        <v>160</v>
+      </c>
+      <c r="D64" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>161</v>
+      </c>
+      <c r="B65" t="s">
+        <v>161</v>
+      </c>
+      <c r="C65" t="s">
+        <v>162</v>
+      </c>
+      <c r="D65" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>163</v>
+      </c>
+      <c r="B66" t="s">
+        <v>163</v>
+      </c>
+      <c r="C66" t="s">
+        <v>164</v>
+      </c>
+      <c r="D66" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>165</v>
+      </c>
+      <c r="B67" t="s">
+        <v>165</v>
+      </c>
+      <c r="C67" t="s">
+        <v>166</v>
+      </c>
+      <c r="D67" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>167</v>
+      </c>
+      <c r="B68" t="s">
+        <v>167</v>
+      </c>
+      <c r="C68" t="s">
+        <v>168</v>
+      </c>
+      <c r="D68" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>179</v>
+      </c>
+      <c r="B69" t="s">
+        <v>182</v>
+      </c>
+      <c r="C69" t="s">
+        <v>171</v>
+      </c>
+      <c r="D69" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>180</v>
+      </c>
+      <c r="B70" t="s">
+        <v>183</v>
+      </c>
+      <c r="C70" t="s">
+        <v>170</v>
+      </c>
+      <c r="D70" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>181</v>
+      </c>
+      <c r="B71" t="s">
+        <v>184</v>
+      </c>
+      <c r="C71" t="s">
+        <v>169</v>
+      </c>
+      <c r="D71" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>